<commit_message>
add proton affinity analysis
</commit_message>
<xml_diff>
--- a/proton_afinity_data.xlsx
+++ b/proton_afinity_data.xlsx
@@ -19,7 +19,7 @@
     <t>Substituent</t>
   </si>
   <si>
-    <t>Proton Afinity</t>
+    <t>Proton Affinity</t>
   </si>
   <si>
     <t>N(CH₃)₂</t>
@@ -522,7 +522,7 @@
         <v>2</v>
       </c>
       <c r="B2">
-        <v>-370.9101145400001</v>
+        <v>-0.591091816</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -530,7 +530,7 @@
         <v>3</v>
       </c>
       <c r="B3">
-        <v>-367.6073718274999</v>
+        <v>-0.585828481</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -538,7 +538,7 @@
         <v>4</v>
       </c>
       <c r="B4">
-        <v>-327.8188970075</v>
+        <v>-0.522420553</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -546,7 +546,7 @@
         <v>5</v>
       </c>
       <c r="B5">
-        <v>-355.104816475</v>
+        <v>-0.56590409</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -554,7 +554,7 @@
         <v>6</v>
       </c>
       <c r="B6">
-        <v>-353.990459305</v>
+        <v>-0.564128222</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -562,7 +562,7 @@
         <v>7</v>
       </c>
       <c r="B7">
-        <v>-363.6779467475</v>
+        <v>-0.579566449</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -570,7 +570,7 @@
         <v>8</v>
       </c>
       <c r="B8">
-        <v>-362.6330776725</v>
+        <v>-0.577901319</v>
       </c>
     </row>
     <row r="9" spans="1:2">
@@ -578,7 +578,7 @@
         <v>9</v>
       </c>
       <c r="B9">
-        <v>-329.4570403499999</v>
+        <v>-0.52503114</v>
       </c>
     </row>
     <row r="10" spans="1:2">
@@ -586,7 +586,7 @@
         <v>10</v>
       </c>
       <c r="B10">
-        <v>-351.82187829</v>
+        <v>-0.560672316</v>
       </c>
     </row>
     <row r="11" spans="1:2">
@@ -594,7 +594,7 @@
         <v>11</v>
       </c>
       <c r="B11">
-        <v>-376.112728335</v>
+        <v>-0.599382834</v>
       </c>
     </row>
     <row r="12" spans="1:2">
@@ -602,7 +602,7 @@
         <v>12</v>
       </c>
       <c r="B12">
-        <v>-375.2777285175</v>
+        <v>-0.598052157</v>
       </c>
     </row>
     <row r="13" spans="1:2">
@@ -610,7 +610,7 @@
         <v>13</v>
       </c>
       <c r="B13">
-        <v>-365.322657505</v>
+        <v>-0.582187502</v>
       </c>
     </row>
     <row r="14" spans="1:2">
@@ -642,7 +642,7 @@
         <v>17</v>
       </c>
       <c r="B17">
-        <v>-318.1446203225</v>
+        <v>-0.507003379</v>
       </c>
     </row>
     <row r="18" spans="1:2">
@@ -650,7 +650,7 @@
         <v>18</v>
       </c>
       <c r="B18">
-        <v>-316.2344676525</v>
+        <v>-0.503959311</v>
       </c>
     </row>
     <row r="19" spans="1:2">
@@ -658,7 +658,7 @@
         <v>19</v>
       </c>
       <c r="B19">
-        <v>-361.3318761025</v>
+        <v>-0.575827691</v>
       </c>
     </row>
     <row r="20" spans="1:2">
@@ -666,7 +666,7 @@
         <v>20</v>
       </c>
       <c r="B20">
-        <v>-327.04407193</v>
+        <v>-0.521185772</v>
       </c>
     </row>
     <row r="21" spans="1:2">
@@ -674,7 +674,7 @@
         <v>21</v>
       </c>
       <c r="B21">
-        <v>-356.4398760625</v>
+        <v>-0.568031675</v>
       </c>
     </row>
     <row r="22" spans="1:2">
@@ -754,7 +754,7 @@
         <v>31</v>
       </c>
       <c r="B31">
-        <v>-351.6785930575001</v>
+        <v>-0.560443973</v>
       </c>
     </row>
     <row r="32" spans="1:2">
@@ -762,7 +762,7 @@
         <v>32</v>
       </c>
       <c r="B32">
-        <v>-357.6837831175</v>
+        <v>-0.570013997</v>
       </c>
     </row>
     <row r="33" spans="1:2">
@@ -770,7 +770,7 @@
         <v>33</v>
       </c>
       <c r="B33">
-        <v>-350.91280649</v>
+        <v>-0.559223596</v>
       </c>
     </row>
     <row r="34" spans="1:2">
@@ -778,7 +778,7 @@
         <v>34</v>
       </c>
       <c r="B34">
-        <v>-359.33624852</v>
+        <v>-0.572647408</v>
       </c>
     </row>
     <row r="35" spans="1:2">
@@ -786,7 +786,7 @@
         <v>35</v>
       </c>
       <c r="B35">
-        <v>-359.6114129175</v>
+        <v>-0.573085917</v>
       </c>
     </row>
     <row r="36" spans="1:2">
@@ -794,7 +794,7 @@
         <v>36</v>
       </c>
       <c r="B36">
-        <v>-357.16739517</v>
+        <v>-0.569191068</v>
       </c>
     </row>
     <row r="37" spans="1:2">
@@ -802,7 +802,7 @@
         <v>37</v>
       </c>
       <c r="B37">
-        <v>-362.0368284275</v>
+        <v>-0.576951121</v>
       </c>
     </row>
     <row r="38" spans="1:2">
@@ -810,7 +810,7 @@
         <v>38</v>
       </c>
       <c r="B38">
-        <v>-365.8528642575</v>
+        <v>-0.583032453</v>
       </c>
     </row>
     <row r="39" spans="1:2">
@@ -818,7 +818,7 @@
         <v>39</v>
       </c>
       <c r="B39">
-        <v>-334.3135515</v>
+        <v>-0.5327706</v>
       </c>
     </row>
     <row r="40" spans="1:2">
@@ -826,7 +826,7 @@
         <v>40</v>
       </c>
       <c r="B40">
-        <v>-365.6452634125</v>
+        <v>-0.582701615</v>
       </c>
     </row>
     <row r="41" spans="1:2">
@@ -834,7 +834,7 @@
         <v>41</v>
       </c>
       <c r="B41">
-        <v>-368.42444648</v>
+        <v>-0.587130592</v>
       </c>
     </row>
     <row r="42" spans="1:2">
@@ -842,7 +842,7 @@
         <v>42</v>
       </c>
       <c r="B42">
-        <v>-362.3977601525</v>
+        <v>-0.577526311</v>
       </c>
     </row>
     <row r="43" spans="1:2">
@@ -850,7 +850,7 @@
         <v>43</v>
       </c>
       <c r="B43">
-        <v>-361.8713303225</v>
+        <v>-0.576687379</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
modified ml models with proton affinity
</commit_message>
<xml_diff>
--- a/proton_afinity_data.xlsx
+++ b/proton_afinity_data.xlsx
@@ -14,12 +14,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="45">
   <si>
     <t>Substituent</t>
   </si>
   <si>
-    <t>Proton Affinity</t>
+    <t>Proton Afinity</t>
+  </si>
+  <si>
+    <t>Std Proton Afinity</t>
   </si>
   <si>
     <t>N(CH₃)₂</t>
@@ -503,354 +506,483 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B43"/>
+  <dimension ref="A1:C43"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:2">
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
       <c r="A2" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B2">
         <v>-0.591091816</v>
       </c>
-    </row>
-    <row r="3" spans="1:2">
+      <c r="C2">
+        <v>-1.007937091</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
       <c r="A3" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B3">
         <v>-0.585828481</v>
       </c>
-    </row>
-    <row r="4" spans="1:2">
+      <c r="C3">
+        <v>-0.8047212419999999</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
       <c r="A4" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B4">
         <v>-0.522420553</v>
       </c>
-    </row>
-    <row r="5" spans="1:2">
+      <c r="C4">
+        <v>1.643440602</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
       <c r="A5" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B5">
         <v>-0.56590409</v>
       </c>
-    </row>
-    <row r="6" spans="1:2">
+      <c r="C5">
+        <v>-0.035446242</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
       <c r="A6" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B6">
         <v>-0.564128222</v>
       </c>
-    </row>
-    <row r="7" spans="1:2">
+      <c r="C6">
+        <v>0.03311951</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
       <c r="A7" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B7">
         <v>-0.579566449</v>
       </c>
-    </row>
-    <row r="8" spans="1:2">
+      <c r="C7">
+        <v>-0.562945989</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
       <c r="A8" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B8">
         <v>-0.577901319</v>
       </c>
-    </row>
-    <row r="9" spans="1:2">
+      <c r="C8">
+        <v>-0.498655799</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
       <c r="A9" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B9">
         <v>-0.52503114</v>
       </c>
-    </row>
-    <row r="10" spans="1:2">
+      <c r="C9">
+        <v>1.542646589</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
       <c r="A10" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B10">
         <v>-0.560672316</v>
       </c>
-    </row>
-    <row r="11" spans="1:2">
+      <c r="C10">
+        <v>0.166551046</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
       <c r="A11" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B11">
         <v>-0.599382834</v>
       </c>
-    </row>
-    <row r="12" spans="1:2">
+      <c r="C11">
+        <v>-1.328050909</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
       <c r="A12" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B12">
         <v>-0.598052157</v>
       </c>
-    </row>
-    <row r="13" spans="1:2">
+      <c r="C12">
+        <v>-1.276673853</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
       <c r="A13" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B13">
         <v>-0.582187502</v>
       </c>
-    </row>
-    <row r="14" spans="1:2">
+      <c r="C13">
+        <v>-0.664144091</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
       <c r="A14" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B14">
         <v>0</v>
       </c>
-    </row>
-    <row r="15" spans="1:2">
+      <c r="C14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
       <c r="A15" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B15">
         <v>0</v>
       </c>
-    </row>
-    <row r="16" spans="1:2">
+      <c r="C15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3">
       <c r="A16" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B16">
         <v>0</v>
       </c>
-    </row>
-    <row r="17" spans="1:2">
+      <c r="C16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
       <c r="A17" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B17">
         <v>-0.507003379</v>
       </c>
-    </row>
-    <row r="18" spans="1:2">
+      <c r="C17">
+        <v>2.238693251</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
       <c r="A18" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B18">
         <v>-0.503959311</v>
       </c>
-    </row>
-    <row r="19" spans="1:2">
+      <c r="C18">
+        <v>2.35622384</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
       <c r="A19" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B19">
         <v>-0.575827691</v>
       </c>
-    </row>
-    <row r="20" spans="1:2">
+      <c r="C19">
+        <v>-0.418593619</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3">
       <c r="A20" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B20">
         <v>-0.521185772</v>
       </c>
-    </row>
-    <row r="21" spans="1:2">
+      <c r="C20">
+        <v>1.69111514</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3">
       <c r="A21" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B21">
         <v>-0.568031675</v>
       </c>
-    </row>
-    <row r="22" spans="1:2">
+      <c r="C21">
+        <v>-0.117591686</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3">
       <c r="A22" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B22">
         <v>0</v>
       </c>
-    </row>
-    <row r="23" spans="1:2">
+      <c r="C22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3">
       <c r="A23" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B23">
         <v>0</v>
       </c>
-    </row>
-    <row r="24" spans="1:2">
+      <c r="C23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3">
       <c r="A24" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B24">
         <v>0</v>
       </c>
-    </row>
-    <row r="25" spans="1:2">
+      <c r="C24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3">
       <c r="A25" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B25">
         <v>0</v>
       </c>
-    </row>
-    <row r="26" spans="1:2">
+      <c r="C25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3">
       <c r="A26" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B26">
         <v>0</v>
       </c>
-    </row>
-    <row r="27" spans="1:2">
+      <c r="C26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3">
       <c r="A27" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B27">
         <v>0</v>
       </c>
-    </row>
-    <row r="28" spans="1:2">
+      <c r="C27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3">
       <c r="A28" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B28">
         <v>0</v>
       </c>
-    </row>
-    <row r="29" spans="1:2">
+      <c r="C28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3">
       <c r="A29" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B29">
         <v>0</v>
       </c>
-    </row>
-    <row r="30" spans="1:2">
+      <c r="C29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3">
       <c r="A30" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B30">
         <v>0</v>
       </c>
-    </row>
-    <row r="31" spans="1:2">
+      <c r="C30">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3">
       <c r="A31" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B31">
         <v>-0.560443973</v>
       </c>
-    </row>
-    <row r="32" spans="1:2">
+      <c r="C31">
+        <v>0.175367303</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3">
       <c r="A32" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B32">
         <v>-0.570013997</v>
       </c>
-    </row>
-    <row r="33" spans="1:2">
+      <c r="C32">
+        <v>-0.194128568</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3">
       <c r="A33" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B33">
         <v>-0.559223596</v>
       </c>
-    </row>
-    <row r="34" spans="1:2">
+      <c r="C33">
+        <v>0.222485708</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3">
       <c r="A34" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B34">
         <v>-0.572647408</v>
       </c>
-    </row>
-    <row r="35" spans="1:2">
+      <c r="C34">
+        <v>-0.295803808</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3">
       <c r="A35" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B35">
         <v>-0.573085917</v>
       </c>
-    </row>
-    <row r="36" spans="1:2">
+      <c r="C35">
+        <v>-0.312734515</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3">
       <c r="A36" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B36">
         <v>-0.569191068</v>
       </c>
-    </row>
-    <row r="37" spans="1:2">
+      <c r="C36">
+        <v>-0.162355516</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3">
       <c r="A37" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B37">
         <v>-0.576951121</v>
       </c>
-    </row>
-    <row r="38" spans="1:2">
+      <c r="C37">
+        <v>-0.461968928</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3">
       <c r="A38" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B38">
         <v>-0.583032453</v>
       </c>
-    </row>
-    <row r="39" spans="1:2">
+      <c r="C38">
+        <v>-0.696767406</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3">
       <c r="A39" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B39">
         <v>-0.5327706</v>
       </c>
-    </row>
-    <row r="40" spans="1:2">
+      <c r="C39">
+        <v>1.243828267</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3">
       <c r="A40" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B40">
         <v>-0.582701615</v>
       </c>
-    </row>
-    <row r="41" spans="1:2">
+      <c r="C40">
+        <v>-0.683993846</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3">
       <c r="A41" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B41">
         <v>-0.587130592</v>
       </c>
-    </row>
-    <row r="42" spans="1:2">
+      <c r="C41">
+        <v>-0.8549953729999999</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3">
       <c r="A42" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B42">
         <v>-0.577526311</v>
       </c>
-    </row>
-    <row r="43" spans="1:2">
+      <c r="C42">
+        <v>-0.484176849</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3">
       <c r="A43" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B43">
         <v>-0.576687379</v>
+      </c>
+      <c r="C43">
+        <v>-0.451785926</v>
       </c>
     </row>
   </sheetData>

</xml_diff>